<commit_message>
Add model RTEDCFG for RTED config
</commit_message>
<xml_diff>
--- a/ams/cases/ieee39/ieee39_esd1.xlsx
+++ b/ams/cases/ieee39/ieee39_esd1.xlsx
@@ -8,32 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F4B68C-86CB-964C-B5AE-B49325274040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773B43B-E676-B444-9056-96B892AEDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="14" r:id="rId1"/>
     <sheet name="Bus" sheetId="1" r:id="rId2"/>
     <sheet name="PQ" sheetId="2" r:id="rId3"/>
     <sheet name="Slack" sheetId="4" r:id="rId4"/>
-    <sheet name="PV" sheetId="3" r:id="rId5"/>
-    <sheet name="ESD1" sheetId="11" r:id="rId6"/>
-    <sheet name="Line" sheetId="5" r:id="rId7"/>
-    <sheet name="Area" sheetId="7" r:id="rId8"/>
-    <sheet name="Region" sheetId="8" r:id="rId9"/>
-    <sheet name="SFR" sheetId="9" r:id="rId10"/>
-    <sheet name="SFRCost" sheetId="10" r:id="rId11"/>
-    <sheet name="GCost" sheetId="6" r:id="rId12"/>
-    <sheet name="EDTSlot" sheetId="12" r:id="rId13"/>
-    <sheet name="UCTSlot" sheetId="13" r:id="rId14"/>
+    <sheet name="RTEDCFG" sheetId="15" r:id="rId5"/>
+    <sheet name="PV" sheetId="3" r:id="rId6"/>
+    <sheet name="ESD1" sheetId="11" r:id="rId7"/>
+    <sheet name="Line" sheetId="5" r:id="rId8"/>
+    <sheet name="Area" sheetId="7" r:id="rId9"/>
+    <sheet name="Region" sheetId="8" r:id="rId10"/>
+    <sheet name="SFR" sheetId="9" r:id="rId11"/>
+    <sheet name="SFRCost" sheetId="10" r:id="rId12"/>
+    <sheet name="GCost" sheetId="6" r:id="rId13"/>
+    <sheet name="EDTSlot" sheetId="12" r:id="rId14"/>
+    <sheet name="UCTSlot" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="392">
   <si>
     <t>idx</t>
   </si>
@@ -1328,14 +1329,24 @@
   <si>
     <t>PV_39</t>
   </si>
+  <si>
+    <t>RTEDCFG1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1467,30 +1478,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1839,6 +1851,77 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1076654-EF34-CC4B-89BB-5D9DC73428FE}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F77866-C777-0B41-8C14-27D8C9A5BF9B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1945,7 +2028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE302B1E-1C21-5545-8C07-A8652D0B6F47}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2143,12 +2226,12 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2545,744 +2628,895 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7E68EB-A0F6-9442-8602-C20717626DB0}">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="172" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16">
-      <c r="A2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="D2" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16">
-      <c r="A3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="D3" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16">
-      <c r="A4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="D4" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="D5" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="D6" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="D7" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D8" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="D9" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="D10" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" t="s">
-        <v>259</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="D11" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16">
-      <c r="A12" t="s">
-        <v>260</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D12" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" t="s">
-        <v>324</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="D13" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" t="s">
-        <v>326</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="D14" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16">
-      <c r="A15" t="s">
-        <v>328</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="D15" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16">
-      <c r="A16" t="s">
-        <v>330</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D16" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16">
-      <c r="A17" t="s">
-        <v>332</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="D17" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16">
-      <c r="A18" t="s">
-        <v>334</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="D18" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16">
-      <c r="A19" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="D19" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16">
-      <c r="A20" t="s">
-        <v>338</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D20" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16">
-      <c r="A21" t="s">
-        <v>340</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="D21" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16">
-      <c r="A22" t="s">
-        <v>342</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="D22" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16">
-      <c r="A23" t="s">
-        <v>344</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="D23" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16">
-      <c r="A24" t="s">
-        <v>346</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D24" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16">
-      <c r="A25" t="s">
-        <v>348</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="D25" s="2">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48AD92-083E-E846-8F62-C9A43521848F}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7E68EB-A0F6-9442-8602-C20717626DB0}">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScale="172" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="16">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16">
+    <row r="2" spans="1:5" ht="16">
       <c r="A2" t="s">
         <v>261</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" t="s">
         <v>251</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" t="s">
         <v>252</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16">
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" t="s">
         <v>253</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C5" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16">
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" t="s">
         <v>254</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C6" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" t="s">
         <v>255</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C7" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16">
+    <row r="8" spans="1:5" ht="16">
       <c r="A8" t="s">
         <v>256</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="C8" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" t="s">
         <v>257</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="C9" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" t="s">
         <v>258</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="C10" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16">
+    <row r="11" spans="1:5" ht="16">
       <c r="A11" t="s">
         <v>259</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="C11" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" t="s">
         <v>260</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="C12" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16">
+    <row r="13" spans="1:5" ht="16">
       <c r="A13" t="s">
         <v>324</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="C13" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" t="s">
         <v>326</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C14" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16">
+    <row r="15" spans="1:5" ht="16">
       <c r="A15" t="s">
         <v>328</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C15" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16">
+    <row r="16" spans="1:5" ht="16">
       <c r="A16" t="s">
         <v>330</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16">
+    <row r="17" spans="1:5" ht="16">
       <c r="A17" t="s">
         <v>332</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C17" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16">
+    <row r="18" spans="1:5" ht="16">
       <c r="A18" t="s">
         <v>334</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="C18" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16">
+    <row r="19" spans="1:5" ht="16">
       <c r="A19" t="s">
         <v>336</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C19" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16">
+    <row r="20" spans="1:5" ht="16">
       <c r="A20" t="s">
         <v>338</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C20" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16">
+    <row r="21" spans="1:5" ht="16">
       <c r="A21" t="s">
         <v>340</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="C21" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E21" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16">
+    <row r="22" spans="1:5" ht="16">
       <c r="A22" t="s">
         <v>342</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C22" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16">
+    <row r="23" spans="1:5" ht="16">
       <c r="A23" t="s">
         <v>344</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="C23" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E23" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16">
+    <row r="24" spans="1:5" ht="16">
       <c r="A24" t="s">
         <v>346</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="C24" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E24" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16">
+    <row r="25" spans="1:5" ht="16">
       <c r="A25" t="s">
         <v>348</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E25" s="2">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48AD92-083E-E846-8F62-C9A43521848F}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E8" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E9" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E10" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E12" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16">
+      <c r="A13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E13" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16">
+      <c r="A14" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E14" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16">
+      <c r="A15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="E15" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16">
+      <c r="A16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E16" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E18" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="E19" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E20" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16">
+      <c r="A21" t="s">
+        <v>340</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E21" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16">
+      <c r="A22" t="s">
+        <v>342</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E22" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16">
+      <c r="A23" t="s">
+        <v>344</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16">
+      <c r="A24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E24" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16">
+      <c r="A25" t="s">
+        <v>348</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="D25" s="2">
+      <c r="E25" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16">
+    <row r="26" spans="1:5" ht="16">
       <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5673,7 +5907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
@@ -5894,6 +6128,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396C59AC-6247-9647-AF4E-4140A33E5886}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16">
+      <c r="A2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
@@ -6915,17 +7192,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BCC95A-1DD8-CE44-8FDD-00EA1DD0739C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7012,7 +7289,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="6">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -7020,7 +7297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
@@ -10805,7 +11082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D9F343-EA84-104D-B986-691ADB4C355F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -10874,75 +11151,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1076654-EF34-CC4B-89BB-5D9DC73428FE}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix dth in RTED objective
</commit_message>
<xml_diff>
--- a/ams/cases/ieee39/ieee39_esd1.xlsx
+++ b/ams/cases/ieee39/ieee39_esd1.xlsx
@@ -8,33 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773B43B-E676-B444-9056-96B892AEDD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464C7384-1BE1-E44F-96FE-E01FAD66097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="14" r:id="rId1"/>
     <sheet name="Bus" sheetId="1" r:id="rId2"/>
     <sheet name="PQ" sheetId="2" r:id="rId3"/>
     <sheet name="Slack" sheetId="4" r:id="rId4"/>
-    <sheet name="RTEDCFG" sheetId="15" r:id="rId5"/>
-    <sheet name="PV" sheetId="3" r:id="rId6"/>
-    <sheet name="ESD1" sheetId="11" r:id="rId7"/>
-    <sheet name="Line" sheetId="5" r:id="rId8"/>
-    <sheet name="Area" sheetId="7" r:id="rId9"/>
-    <sheet name="Region" sheetId="8" r:id="rId10"/>
-    <sheet name="SFR" sheetId="9" r:id="rId11"/>
-    <sheet name="SFRCost" sheetId="10" r:id="rId12"/>
-    <sheet name="GCost" sheetId="6" r:id="rId13"/>
-    <sheet name="EDTSlot" sheetId="12" r:id="rId14"/>
-    <sheet name="UCTSlot" sheetId="13" r:id="rId15"/>
+    <sheet name="PV" sheetId="3" r:id="rId5"/>
+    <sheet name="ESD1" sheetId="11" r:id="rId6"/>
+    <sheet name="Line" sheetId="5" r:id="rId7"/>
+    <sheet name="Area" sheetId="7" r:id="rId8"/>
+    <sheet name="Region" sheetId="8" r:id="rId9"/>
+    <sheet name="SFR" sheetId="9" r:id="rId10"/>
+    <sheet name="SFRCost" sheetId="10" r:id="rId11"/>
+    <sheet name="GCost" sheetId="6" r:id="rId12"/>
+    <sheet name="EDTSlot" sheetId="12" r:id="rId13"/>
+    <sheet name="UCTSlot" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="390">
   <si>
     <t>idx</t>
   </si>
@@ -1052,9 +1051,6 @@
     <t>sd</t>
   </si>
   <si>
-    <t>dt</t>
-  </si>
-  <si>
     <t>EDT1</t>
   </si>
   <si>
@@ -1328,25 +1324,15 @@
   </si>
   <si>
     <t>PV_39</t>
-  </si>
-  <si>
-    <t>RTEDCFG1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1478,31 +1464,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1820,16 +1805,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
@@ -1837,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>379</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>380</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1851,77 +1836,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1076654-EF34-CC4B-89BB-5D9DC73428FE}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F77866-C777-0B41-8C14-27D8C9A5BF9B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -2028,7 +1942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE302B1E-1C21-5545-8C07-A8652D0B6F47}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2063,7 +1977,7 @@
         <v>275</v>
       </c>
       <c r="C2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D2" t="s">
         <v>261</v>
@@ -2080,7 +1994,7 @@
         <v>276</v>
       </c>
       <c r="C3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D3" t="s">
         <v>261</v>
@@ -2097,7 +2011,7 @@
         <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D4" t="s">
         <v>261</v>
@@ -2114,7 +2028,7 @@
         <v>278</v>
       </c>
       <c r="C5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D5" t="s">
         <v>261</v>
@@ -2131,7 +2045,7 @@
         <v>279</v>
       </c>
       <c r="C6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D6" t="s">
         <v>261</v>
@@ -2148,7 +2062,7 @@
         <v>280</v>
       </c>
       <c r="C7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D7" t="s">
         <v>261</v>
@@ -2165,7 +2079,7 @@
         <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D8" t="s">
         <v>261</v>
@@ -2182,7 +2096,7 @@
         <v>282</v>
       </c>
       <c r="C9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D9" t="s">
         <v>261</v>
@@ -2199,7 +2113,7 @@
         <v>283</v>
       </c>
       <c r="C10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D10" t="s">
         <v>261</v>
@@ -2216,7 +2130,7 @@
         <v>284</v>
       </c>
       <c r="C11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D11" t="s">
         <v>261</v>
@@ -2226,12 +2140,12 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2291,7 +2205,7 @@
         <v>250</v>
       </c>
       <c r="E2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -2326,7 +2240,7 @@
         <v>240</v>
       </c>
       <c r="E3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -2361,7 +2275,7 @@
         <v>241</v>
       </c>
       <c r="E4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2396,7 +2310,7 @@
         <v>242</v>
       </c>
       <c r="E5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2431,7 +2345,7 @@
         <v>243</v>
       </c>
       <c r="E6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -2466,7 +2380,7 @@
         <v>244</v>
       </c>
       <c r="E7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -2501,7 +2415,7 @@
         <v>245</v>
       </c>
       <c r="E8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -2536,7 +2450,7 @@
         <v>246</v>
       </c>
       <c r="E9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -2571,7 +2485,7 @@
         <v>247</v>
       </c>
       <c r="E10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -2606,7 +2520,7 @@
         <v>248</v>
       </c>
       <c r="E11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2628,22 +2542,388 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7E68EB-A0F6-9442-8602-C20717626DB0}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16">
+      <c r="A2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16">
+      <c r="A3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" t="s">
+        <v>329</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16">
+      <c r="A18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16">
+      <c r="A19" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16">
+      <c r="A20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16">
+      <c r="A21" t="s">
+        <v>339</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16">
+      <c r="A22" t="s">
+        <v>341</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" t="s">
+        <v>343</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16">
+      <c r="A24" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16">
+      <c r="A25" t="s">
+        <v>347</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7E68EB-A0F6-9442-8602-C20717626DB0}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48AD92-083E-E846-8F62-C9A43521848F}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="172" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2656,867 +2936,350 @@
       <c r="D1" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+    </row>
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" t="s">
         <v>261</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="E2" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16">
+    </row>
+    <row r="3" spans="1:4" ht="16">
       <c r="A3" t="s">
         <v>251</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="E3" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16">
+    </row>
+    <row r="4" spans="1:4" ht="16">
       <c r="A4" t="s">
         <v>252</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="E4" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16">
+    </row>
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" t="s">
         <v>253</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E5" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16">
+    </row>
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" t="s">
         <v>254</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E6" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16">
+    </row>
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" t="s">
         <v>255</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="E7" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
+    </row>
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" t="s">
         <v>256</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>357</v>
+        <v>318</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>357</v>
+        <v>318</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="E8" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" t="s">
         <v>257</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>358</v>
+        <v>319</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>358</v>
+        <v>319</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E9" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" t="s">
         <v>258</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>359</v>
+        <v>320</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>359</v>
+        <v>320</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="E10" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" t="s">
         <v>259</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>360</v>
+        <v>321</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>360</v>
+        <v>321</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E11" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" t="s">
         <v>260</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>361</v>
+        <v>322</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>361</v>
+        <v>322</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" t="s">
+        <v>329</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16">
+      <c r="A18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16">
+      <c r="A19" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16">
+      <c r="A20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16">
+      <c r="A21" t="s">
+        <v>339</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="E12" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16">
-      <c r="A13" t="s">
-        <v>324</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E13" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16">
-      <c r="A14" t="s">
-        <v>326</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="E14" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16">
-      <c r="A15" t="s">
-        <v>328</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="E15" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16">
-      <c r="A16" t="s">
-        <v>330</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="E16" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16">
-      <c r="A17" t="s">
-        <v>332</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E17" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16">
-      <c r="A18" t="s">
-        <v>334</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E18" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16">
-      <c r="A19" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="E19" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16">
-      <c r="A20" t="s">
-        <v>338</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="D20" s="8" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="16">
+      <c r="A22" t="s">
+        <v>341</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" t="s">
+        <v>343</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="E20" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16">
-      <c r="A21" t="s">
-        <v>340</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E21" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16">
-      <c r="A22" t="s">
-        <v>342</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="D22" s="8" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="16">
+      <c r="A24" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16">
+      <c r="A25" t="s">
+        <v>347</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="E22" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16">
-      <c r="A23" t="s">
-        <v>344</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E23" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16">
-      <c r="A24" t="s">
-        <v>346</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="E24" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="16">
-      <c r="A25" t="s">
-        <v>348</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E25" s="2">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48AD92-083E-E846-8F62-C9A43521848F}">
-  <dimension ref="A1:E26"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
-      <c r="A2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="E2" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16">
-      <c r="A3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="E3" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16">
-      <c r="A4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="E4" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16">
-      <c r="A5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E5" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16">
-      <c r="A6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E6" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16">
-      <c r="A7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="E7" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16">
-      <c r="A8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="E8" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16">
-      <c r="A9" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E9" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16">
-      <c r="A10" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="E10" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16">
-      <c r="A11" t="s">
-        <v>259</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E11" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16">
-      <c r="A12" t="s">
-        <v>260</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="E12" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16">
-      <c r="A13" t="s">
-        <v>324</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E13" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16">
-      <c r="A14" t="s">
-        <v>326</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="E14" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16">
-      <c r="A15" t="s">
-        <v>328</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="E15" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16">
-      <c r="A16" t="s">
-        <v>330</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="E16" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16">
-      <c r="A17" t="s">
-        <v>332</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="E17" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16">
-      <c r="A18" t="s">
-        <v>334</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E18" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16">
-      <c r="A19" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="E19" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16">
-      <c r="A20" t="s">
-        <v>338</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="E20" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="16">
-      <c r="A21" t="s">
-        <v>340</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E21" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="16">
-      <c r="A22" t="s">
-        <v>342</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="E22" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16">
-      <c r="A23" t="s">
-        <v>344</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E23" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="16">
-      <c r="A24" t="s">
-        <v>346</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="E24" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="16">
-      <c r="A25" t="s">
-        <v>348</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E25" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="16">
+    </row>
+    <row r="26" spans="1:4" ht="16">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6023,13 +5786,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -6128,49 +5891,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396C59AC-6247-9647-AF4E-4140A33E5886}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16">
-      <c r="A2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>391</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>391</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
@@ -6287,13 +6007,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -6388,13 +6108,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -6489,13 +6209,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -6590,13 +6310,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -6691,13 +6411,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -6792,13 +6512,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -6893,13 +6613,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -6994,13 +6714,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -7095,13 +6815,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -7192,16 +6912,16 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BCC95A-1DD8-CE44-8FDD-00EA1DD0739C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+    <sheetView zoomScale="158" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -7268,7 +6988,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G2" s="6">
         <v>100</v>
@@ -7297,7 +7017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
@@ -11082,7 +10802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D9F343-EA84-104D-B986-691ADB4C355F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -11151,4 +10871,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1076654-EF34-CC4B-89BB-5D9DC73428FE}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>